<commit_message>
Add new test case edit profile, delete blog from user profile
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_BaoTran\pHpDemo\src\test\java\pHpFox\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C20E267-69DE-4FEA-8063-90ED42C82E66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3A932E-7EFD-413D-B198-D2E56EE1C6A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="131">
   <si>
     <t>id</t>
   </si>
@@ -989,7 +989,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1968,11 +1968,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC1001"/>
+  <dimension ref="A1:AB1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1982,10 +1982,11 @@
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="48.5703125" customWidth="1"/>
     <col min="9" max="9" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2007,12 +2008,10 @@
       <c r="G1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>107</v>
       </c>
+      <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -2032,9 +2031,8 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="15" t="s">
@@ -2052,12 +2050,11 @@
       <c r="G2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15" t="s">
@@ -2075,12 +2072,11 @@
       <c r="G3" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="15" t="s">
@@ -2098,12 +2094,11 @@
       <c r="G4" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="16" t="s">
+      <c r="H4" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="15" t="s">
@@ -2121,12 +2116,11 @@
       <c r="G5" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="15" t="s">
@@ -2144,39 +2138,38 @@
       <c r="G6" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="16" t="s">
+      <c r="H6" s="16" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
@@ -5150,11 +5143,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5162,11 +5155,11 @@
     <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5213,8 +5206,67 @@
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
     </row>
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D2" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D3" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="8">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="8">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="8">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D6" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="8">
+        <v>123456</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{A4BBEE31-E0B1-44DD-8789-E4C966FAAD6C}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{47381A3E-A0A2-4665-B64C-1B759005BD25}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug and add new tests: edit profile
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3A932E-7EFD-413D-B198-D2E56EE1C6A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6821300-839C-4A12-8E90-35111EDD4F3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="info" sheetId="1" r:id="rId1"/>
-    <sheet name="video_urls" sheetId="2" r:id="rId2"/>
+    <sheet name="browserConfig" sheetId="1" r:id="rId1"/>
+    <sheet name="blogs" sheetId="2" r:id="rId2"/>
     <sheet name="pages" sheetId="3" r:id="rId3"/>
     <sheet name="users" sheetId="4" r:id="rId4"/>
     <sheet name="photos" sheetId="5" r:id="rId5"/>
@@ -24,6 +24,42 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{BBFBB8E8-3422-4DEE-A4B2-05D2BA15E3DE}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Automation script opens browser in order of priority</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{9C4F1BB9-CBDC-4B96-ADC1-FE6DB56A264F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>do not changed column header</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -59,7 +95,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -95,7 +131,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -131,7 +167,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -168,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="131">
   <si>
     <t>id</t>
   </si>
@@ -197,12 +233,6 @@
     <t>guest</t>
   </si>
   <si>
-    <t>video</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/watch/?v=682500276531720</t>
-  </si>
-  <si>
     <t>sidebar</t>
   </si>
   <si>
@@ -561,6 +591,12 @@
   </si>
   <si>
     <t>/event/add</t>
+  </si>
+  <si>
+    <t>flatform</t>
+  </si>
+  <si>
+    <t>browsername</t>
   </si>
 </sst>
 </file>
@@ -622,7 +658,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -630,12 +666,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -666,6 +717,8 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -881,65 +934,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:AC2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="20" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2"/>
@@ -963,43 +998,69 @@
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
+    <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="21">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+    </row>
+    <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="21">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC83"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1016,7 +1077,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -1048,21 +1109,99 @@
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
     </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:AC83"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+    </row>
     <row r="2" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1070,10 +1209,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1081,10 +1220,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1092,10 +1231,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1103,10 +1242,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1114,10 +1253,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1125,10 +1264,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1136,10 +1275,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1147,10 +1286,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1158,10 +1297,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1169,10 +1308,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1180,10 +1319,10 @@
         <v>3</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1191,10 +1330,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1202,10 +1341,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="12.75" x14ac:dyDescent="0.2">
@@ -1213,10 +1352,10 @@
         <v>3</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1224,10 +1363,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1235,10 +1374,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1246,10 +1385,10 @@
         <v>3</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1257,10 +1396,10 @@
         <v>90</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1268,10 +1407,10 @@
         <v>90</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1279,10 +1418,10 @@
         <v>90</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1290,10 +1429,10 @@
         <v>90</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1301,10 +1440,10 @@
         <v>90</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1312,10 +1451,10 @@
         <v>90</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1323,10 +1462,10 @@
         <v>90</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1334,10 +1473,10 @@
         <v>90</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1345,10 +1484,10 @@
         <v>90</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1356,10 +1495,10 @@
         <v>90</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1367,10 +1506,10 @@
         <v>90</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1378,10 +1517,10 @@
         <v>90</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1389,10 +1528,10 @@
         <v>90</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1400,10 +1539,10 @@
         <v>90</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1411,10 +1550,10 @@
         <v>4</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1422,10 +1561,10 @@
         <v>5</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1433,10 +1572,10 @@
         <v>5</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1444,10 +1583,10 @@
         <v>5</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1455,10 +1594,10 @@
         <v>5</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1466,10 +1605,10 @@
         <v>5</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1477,10 +1616,10 @@
         <v>5</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1488,10 +1627,10 @@
         <v>6</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1499,10 +1638,10 @@
         <v>6</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1510,10 +1649,10 @@
         <v>6</v>
       </c>
       <c r="C43" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1521,10 +1660,10 @@
         <v>6</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1532,10 +1671,10 @@
         <v>6</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1543,10 +1682,10 @@
         <v>6</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1554,10 +1693,10 @@
         <v>7</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1565,10 +1704,10 @@
         <v>7</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1576,10 +1715,10 @@
         <v>7</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1587,10 +1726,10 @@
         <v>7</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1598,10 +1737,10 @@
         <v>7</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1609,10 +1748,10 @@
         <v>8</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1620,10 +1759,10 @@
         <v>8</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1631,10 +1770,10 @@
         <v>8</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1642,10 +1781,10 @@
         <v>8</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1653,10 +1792,10 @@
         <v>8</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1664,10 +1803,10 @@
         <v>8</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1675,10 +1814,10 @@
         <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1686,10 +1825,10 @@
         <v>8</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1697,10 +1836,10 @@
         <v>8</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1708,10 +1847,10 @@
         <v>8</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1719,10 +1858,10 @@
         <v>8</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1730,10 +1869,10 @@
         <v>8</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1741,10 +1880,10 @@
         <v>8</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1752,10 +1891,10 @@
         <v>9</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1763,10 +1902,10 @@
         <v>9</v>
       </c>
       <c r="C66" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="67" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1774,10 +1913,10 @@
         <v>9</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1785,10 +1924,10 @@
         <v>9</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1796,10 +1935,10 @@
         <v>9</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1807,10 +1946,10 @@
         <v>9</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1818,10 +1957,10 @@
         <v>9</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1829,10 +1968,10 @@
         <v>9</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1840,10 +1979,10 @@
         <v>10</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1851,10 +1990,10 @@
         <v>12</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1862,10 +2001,10 @@
         <v>12</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1873,10 +2012,10 @@
         <v>12</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1884,10 +2023,10 @@
         <v>12</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="78" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1895,10 +2034,10 @@
         <v>12</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="2:4" ht="12.75" x14ac:dyDescent="0.2">
@@ -1906,10 +2045,10 @@
         <v>14</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1917,10 +2056,10 @@
         <v>14</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1928,10 +2067,10 @@
         <v>14</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1939,10 +2078,10 @@
         <v>14</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="83" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1950,10 +2089,10 @@
         <v>14</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1972,7 +2111,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1994,22 +2133,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="F1" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -2036,110 +2175,110 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="F2" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="G2" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="14"/>
       <c r="C3" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>93</v>
       </c>
       <c r="F3" s="8">
         <v>123456</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F4" s="8">
         <v>123456</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="14"/>
       <c r="B5" s="14"/>
       <c r="C5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>100</v>
       </c>
       <c r="F5" s="8">
         <v>123456</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>102</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>104</v>
       </c>
       <c r="F6" s="8">
         <v>123456</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -5147,7 +5286,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5167,16 +5306,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -5208,21 +5347,21 @@
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D2" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D3" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F3" s="8">
         <v>123456</v>
@@ -5230,10 +5369,10 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F4" s="8">
         <v>123456</v>
@@ -5241,10 +5380,10 @@
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F5" s="8">
         <v>123456</v>
@@ -5252,10 +5391,10 @@
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F6" s="8">
         <v>123456</v>

</xml_diff>

<commit_message>
Add new test case on Group Module: Process on Secret Group
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6821300-839C-4A12-8E90-35111EDD4F3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76FC7D0-6C65-421A-A135-425E18B8CEEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="134">
   <si>
     <t>id</t>
   </si>
@@ -597,6 +597,15 @@
   </si>
   <si>
     <t>browsername</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test@phpfox.com</t>
+  </si>
+  <si>
+    <t>/test</t>
   </si>
 </sst>
 </file>
@@ -2111,7 +2120,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2282,7 +2291,24 @@
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="F7" s="5"/>
+      <c r="C7" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="5">
+        <v>123456</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F8" s="6"/>

</xml_diff>

<commit_message>
Action on Closed Group
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76FC7D0-6C65-421A-A135-425E18B8CEEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5308331-436F-420E-9C21-D8FA6F4C750A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2120,7 +2120,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2255,7 +2255,7 @@
       <c r="D5" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="17" t="s">
         <v>98</v>
       </c>
       <c r="F5" s="8">
@@ -5296,10 +5296,11 @@
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{503540FC-8460-4D96-A4D6-6C87EEBE8A4E}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{B1AF28E8-005A-4456-9047-1070A5527857}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{69BBBFE8-0E8C-40EC-AB31-020B9243D8BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Action on Poll Vs 0.2: fix bugs and new test script on Event
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5308331-436F-420E-9C21-D8FA6F4C750A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FF2CBB-BE2C-4A69-B266-90396B0BA1C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2120,7 +2120,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add new test script on Forum App- View admin
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FF2CBB-BE2C-4A69-B266-90396B0BA1C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9FF525-6D73-4C63-9DE4-3A22F09ADD2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="135">
   <si>
     <t>id</t>
   </si>
@@ -606,6 +606,9 @@
   </si>
   <si>
     <t>/test</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
@@ -2120,7 +2123,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2214,8 +2217,8 @@
       <c r="E3" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="8">
-        <v>123456</v>
+      <c r="F3" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
change flow test script, add new test script on Photo
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20388"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9FF525-6D73-4C63-9DE4-3A22F09ADD2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3091929F-460E-4F0F-8C78-F76E2B6A7193}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2123,7 +2123,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
change position test case verify UI
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3091929F-460E-4F0F-8C78-F76E2B6A7193}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36368B52-BEC7-442A-A05B-2609FF891205}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2123,7 +2123,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add new test script on Share action
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36368B52-BEC7-442A-A05B-2609FF891205}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7584631E-0AE0-45B6-A00A-ED84C0DCE37D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2123,7 +2123,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
changed condition add comment
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7584631E-0AE0-45B6-A00A-ED84C0DCE37D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BB35E8-E789-482B-B90A-450D67F55A0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2123,7 +2123,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add test case config on ACP
</commit_message>
<xml_diff>
--- a/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
+++ b/src/test/java/MetaFox/testdata/v5DataProvider.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace_BaoTran\pHpDemo\src\test\java\MetaFox\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BB35E8-E789-482B-B90A-450D67F55A0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E37517C-762B-4320-A28E-86E1B38D50D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2123,7 +2123,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>